<commit_message>
valid project owner credentials
</commit_message>
<xml_diff>
--- a/Manual Testing.xlsx
+++ b/Manual Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\sqa projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D513A5A-DDCF-46AE-87A9-6F83D848CECF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D6F63B-9AB1-49BB-AD60-4861D4911552}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="77">
   <si>
     <t>Project Name</t>
   </si>
@@ -235,13 +235,37 @@
 </t>
   </si>
   <si>
-    <t>The placeholder is removed and email  entered successfully and password is encrypted</t>
+    <t xml:space="preserve">Register using valid project owner credentials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
   </si>
   <si>
     <t>Sheikh Asiful Islam</t>
   </si>
   <si>
-    <t xml:space="preserve"> Testing </t>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>click on the project owner radio buttton</t>
+  </si>
+  <si>
+    <t>The project owner button is selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter a valid project owner username </t>
+  </si>
+  <si>
+    <t>The placeholder is removed and email  entered successfully and password is encrypted (****)</t>
+  </si>
+  <si>
+    <t>The placeholder is removed and email  entered successfully and password is encrypted (***)</t>
   </si>
 </sst>
 </file>
@@ -411,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -473,7 +497,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -502,6 +525,10 @@
     <xf numFmtId="49" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -514,107 +541,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1051,8 +985,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1"/>
@@ -1063,89 +997,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="36"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="A1" s="37"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="65.25" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:10" ht="56.25" customHeight="1">
+      <c r="A3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-    </row>
-    <row r="3" spans="1:10" ht="56.25" customHeight="1">
-      <c r="A3" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="55.5" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:10" ht="71.25" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:10" ht="57" customHeight="1">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="J6" s="24"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1167,16 +1101,16 @@
     <tabColor rgb="FFF1C232"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
@@ -1214,7 +1148,7 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="4"/>
@@ -1228,7 +1162,7 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="6"/>
@@ -1242,10 +1176,10 @@
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="31" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -1264,7 +1198,7 @@
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1286,7 +1220,7 @@
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -1305,14 +1239,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="13"/>
@@ -1321,13 +1255,13 @@
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="31" t="s">
         <v>62</v>
       </c>
       <c r="D8" s="9"/>
@@ -1336,26 +1270,32 @@
       <c r="G8" s="13"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+    <row r="9" spans="1:8" s="34" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="5">
         <v>2</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="B9" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" s="34" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>73</v>
+      </c>
       <c r="D10" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="9" t="s">
@@ -1366,12 +1306,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:8" s="34" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A11" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
@@ -1384,12 +1328,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:8" s="34" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A12" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="D12" s="9" t="s">
         <v>16</v>
       </c>
@@ -1402,39 +1350,41 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A13" s="5">
-        <v>3</v>
-      </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
-        <v>16</v>
-      </c>
+    <row r="13" spans="1:8" s="34" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A13" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" s="34" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A14" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="9"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="F14" s="9"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>23</v>
+      <c r="A15" s="41" t="s">
+        <v>71</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="8"/>
@@ -1451,38 +1401,38 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" s="5">
+        <v>4</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17" s="5">
-        <v>4</v>
-      </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
+      <c r="A17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="8"/>
@@ -1500,7 +1450,7 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="8"/>
@@ -1518,10 +1468,10 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1534,93 +1484,85 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="5">
+    <row r="21" spans="1:8">
+      <c r="A21" s="5">
         <v>5</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A23" s="7" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="5"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="5"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" ht="12.75">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="12.75">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:8" ht="12.75">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="5"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" ht="12.75">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" ht="12.75">
       <c r="A28" s="7"/>
@@ -1632,30 +1574,30 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" ht="12.75">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+    <row r="29" spans="1:8">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" ht="12.75">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" ht="12.75">
       <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
       <c r="F31" s="9"/>
@@ -1717,33 +1659,33 @@
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="10"/>
       <c r="F37" s="9"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" ht="12.75">
-      <c r="A38" s="7"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="5"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
+    <row r="38" spans="1:8">
+      <c r="A38" s="5"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" ht="12.75">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="12.75">
       <c r="A40" s="7"/>
-      <c r="B40" s="8"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
@@ -1754,7 +1696,7 @@
     <row r="41" spans="1:8" ht="12.75">
       <c r="A41" s="7"/>
       <c r="B41" s="11"/>
-      <c r="C41" s="8"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
       <c r="F41" s="9"/>
@@ -1801,30 +1743,30 @@
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8" ht="12.75">
-      <c r="A46" s="7"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="5"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+    <row r="46" spans="1:8">
+      <c r="A46" s="5"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" ht="12.75">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" ht="12.75">
       <c r="A48" s="7"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="9"/>
       <c r="E48" s="10"/>
       <c r="F48" s="9"/>
@@ -1844,36 +1786,36 @@
     <row r="50" spans="1:8" ht="12.75">
       <c r="A50" s="7"/>
       <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
+      <c r="C50" s="8"/>
       <c r="D50" s="9"/>
-      <c r="E50" s="10"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-    </row>
-    <row r="51" spans="1:8" ht="12.75">
-      <c r="A51" s="7"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="5"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="5"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" ht="12.75">
+      <c r="A52" s="7"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" ht="12.75">
       <c r="A53" s="7"/>
-      <c r="B53" s="8"/>
+      <c r="B53" s="11"/>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
@@ -1894,7 +1836,7 @@
     <row r="55" spans="1:8" ht="12.75">
       <c r="A55" s="7"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="8"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="9"/>
       <c r="E55" s="10"/>
       <c r="F55" s="9"/>
@@ -1904,36 +1846,36 @@
     <row r="56" spans="1:8" ht="12.75">
       <c r="A56" s="7"/>
       <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
+      <c r="C56" s="8"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="10"/>
+      <c r="E56" s="13"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-    </row>
-    <row r="57" spans="1:8" ht="12.75">
-      <c r="A57" s="7"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="5"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="5"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:8" ht="12.75">
+      <c r="A58" s="7"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" ht="12.75">
       <c r="A59" s="7"/>
-      <c r="B59" s="8"/>
+      <c r="B59" s="11"/>
       <c r="C59" s="8"/>
       <c r="D59" s="9"/>
       <c r="E59" s="10"/>
@@ -1954,7 +1896,7 @@
     <row r="61" spans="1:8" ht="12.75">
       <c r="A61" s="7"/>
       <c r="B61" s="11"/>
-      <c r="C61" s="8"/>
+      <c r="C61" s="11"/>
       <c r="D61" s="9"/>
       <c r="E61" s="10"/>
       <c r="F61" s="9"/>
@@ -1964,36 +1906,36 @@
     <row r="62" spans="1:8" ht="12.75">
       <c r="A62" s="7"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
+      <c r="C62" s="8"/>
       <c r="D62" s="9"/>
-      <c r="E62" s="10"/>
+      <c r="E62" s="13"/>
       <c r="F62" s="9"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-    </row>
-    <row r="63" spans="1:8" ht="12.75">
-      <c r="A63" s="7"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="5"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="5"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="1:8" ht="12.75">
+      <c r="A64" s="7"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" ht="12.75">
       <c r="A65" s="7"/>
-      <c r="B65" s="8"/>
+      <c r="B65" s="11"/>
       <c r="C65" s="8"/>
       <c r="D65" s="9"/>
       <c r="E65" s="10"/>
@@ -2014,7 +1956,7 @@
     <row r="67" spans="1:8" ht="12.75">
       <c r="A67" s="7"/>
       <c r="B67" s="11"/>
-      <c r="C67" s="8"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="9"/>
       <c r="E67" s="10"/>
       <c r="F67" s="9"/>
@@ -2036,10 +1978,10 @@
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
       <c r="D69" s="9"/>
-      <c r="E69" s="10"/>
+      <c r="E69" s="13"/>
       <c r="F69" s="9"/>
-      <c r="G69" s="10"/>
-      <c r="H69" s="10"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
     </row>
     <row r="70" spans="1:8" ht="12.75">
       <c r="A70" s="7"/>
@@ -2056,10 +1998,10 @@
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="9"/>
-      <c r="E71" s="13"/>
+      <c r="E71" s="10"/>
       <c r="F71" s="9"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
     </row>
     <row r="72" spans="1:8" ht="12.75">
       <c r="A72" s="7"/>
@@ -2071,29 +2013,29 @@
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="1:8" ht="12.75">
-      <c r="A73" s="7"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="10"/>
-      <c r="H73" s="10"/>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="5"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="38"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
+    <row r="73" spans="1:8">
+      <c r="A73" s="5"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" ht="12.75">
+      <c r="A74" s="7"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
     </row>
     <row r="75" spans="1:8" ht="12.75">
       <c r="A75" s="7"/>
-      <c r="B75" s="8"/>
+      <c r="B75" s="11"/>
       <c r="C75" s="8"/>
       <c r="D75" s="9"/>
       <c r="E75" s="10"/>
@@ -2114,7 +2056,7 @@
     <row r="77" spans="1:8" ht="12.75">
       <c r="A77" s="7"/>
       <c r="B77" s="11"/>
-      <c r="C77" s="8"/>
+      <c r="C77" s="11"/>
       <c r="D77" s="9"/>
       <c r="E77" s="10"/>
       <c r="F77" s="9"/>
@@ -2136,20 +2078,20 @@
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
       <c r="D79" s="9"/>
-      <c r="E79" s="10"/>
+      <c r="E79" s="13"/>
       <c r="F79" s="9"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
     </row>
     <row r="80" spans="1:8" ht="12.75">
       <c r="A80" s="7"/>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
       <c r="D80" s="9"/>
-      <c r="E80" s="13"/>
+      <c r="E80" s="10"/>
       <c r="F80" s="9"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
     </row>
     <row r="81" spans="1:8" ht="12.75">
       <c r="A81" s="7"/>
@@ -2181,30 +2123,30 @@
       <c r="G83" s="10"/>
       <c r="H83" s="10"/>
     </row>
-    <row r="84" spans="1:8" ht="12.75">
-      <c r="A84" s="7"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="10"/>
-      <c r="H84" s="10"/>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="5"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="38"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
-      <c r="G85" s="6"/>
-      <c r="H85" s="6"/>
+    <row r="84" spans="1:8">
+      <c r="A84" s="5"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+    </row>
+    <row r="85" spans="1:8" ht="12.75">
+      <c r="A85" s="7"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
     </row>
     <row r="86" spans="1:8" ht="12.75">
       <c r="A86" s="7"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
       <c r="D86" s="9"/>
       <c r="E86" s="10"/>
       <c r="F86" s="9"/>
@@ -2251,25 +2193,25 @@
       <c r="G90" s="10"/>
       <c r="H90" s="10"/>
     </row>
-    <row r="91" spans="1:8" ht="12.75">
-      <c r="A91" s="7"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="9"/>
-      <c r="G91" s="10"/>
-      <c r="H91" s="10"/>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="5"/>
-      <c r="B92" s="37"/>
-      <c r="C92" s="38"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
+    <row r="91" spans="1:8">
+      <c r="A91" s="5"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+    </row>
+    <row r="92" spans="1:8" ht="12.75">
+      <c r="A92" s="7"/>
+      <c r="B92" s="12"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
     </row>
     <row r="93" spans="1:8" ht="12.75">
       <c r="A93" s="7"/>
@@ -2288,33 +2230,33 @@
       <c r="D94" s="9"/>
       <c r="E94" s="10"/>
       <c r="F94" s="9"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
-    </row>
-    <row r="95" spans="1:8" ht="12.75">
-      <c r="A95" s="7"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="9"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="9"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="5"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="39"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="6"/>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
     </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="5"/>
-      <c r="B96" s="37"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="15"/>
-      <c r="F96" s="6"/>
+    <row r="96" spans="1:8" ht="12.75">
+      <c r="A96" s="7"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="9"/>
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
     </row>
     <row r="97" spans="1:8" ht="12.75">
       <c r="A97" s="7"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="8"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
       <c r="D97" s="9"/>
       <c r="E97" s="16"/>
       <c r="F97" s="9"/>
@@ -2344,7 +2286,7 @@
     <row r="100" spans="1:8" ht="12.75">
       <c r="A100" s="7"/>
       <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
+      <c r="C100" s="8"/>
       <c r="D100" s="9"/>
       <c r="E100" s="16"/>
       <c r="F100" s="9"/>
@@ -2354,7 +2296,7 @@
     <row r="101" spans="1:8" ht="12.75">
       <c r="A101" s="7"/>
       <c r="B101" s="11"/>
-      <c r="C101" s="8"/>
+      <c r="C101" s="11"/>
       <c r="D101" s="9"/>
       <c r="E101" s="16"/>
       <c r="F101" s="9"/>
@@ -2384,7 +2326,7 @@
     <row r="104" spans="1:8" ht="12.75">
       <c r="A104" s="7"/>
       <c r="B104" s="11"/>
-      <c r="C104" s="11"/>
+      <c r="C104" s="8"/>
       <c r="D104" s="9"/>
       <c r="E104" s="16"/>
       <c r="F104" s="9"/>
@@ -2394,7 +2336,7 @@
     <row r="105" spans="1:8" ht="12.75">
       <c r="A105" s="7"/>
       <c r="B105" s="11"/>
-      <c r="C105" s="8"/>
+      <c r="C105" s="11"/>
       <c r="D105" s="9"/>
       <c r="E105" s="16"/>
       <c r="F105" s="9"/>
@@ -2426,7 +2368,7 @@
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="9"/>
-      <c r="E108" s="16"/>
+      <c r="E108" s="17"/>
       <c r="F108" s="9"/>
       <c r="G108" s="13"/>
       <c r="H108" s="13"/>
@@ -2436,7 +2378,7 @@
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
       <c r="D109" s="9"/>
-      <c r="E109" s="17"/>
+      <c r="E109" s="16"/>
       <c r="F109" s="9"/>
       <c r="G109" s="13"/>
       <c r="H109" s="13"/>
@@ -2446,7 +2388,7 @@
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
       <c r="D110" s="9"/>
-      <c r="E110" s="16"/>
+      <c r="E110" s="17"/>
       <c r="F110" s="9"/>
       <c r="G110" s="13"/>
       <c r="H110" s="13"/>
@@ -2456,7 +2398,7 @@
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
       <c r="D111" s="9"/>
-      <c r="E111" s="17"/>
+      <c r="E111" s="16"/>
       <c r="F111" s="9"/>
       <c r="G111" s="13"/>
       <c r="H111" s="13"/>
@@ -2466,55 +2408,58 @@
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
       <c r="D112" s="9"/>
-      <c r="E112" s="16"/>
+      <c r="E112" s="17"/>
       <c r="F112" s="9"/>
       <c r="G112" s="13"/>
       <c r="H112" s="13"/>
     </row>
-    <row r="113" spans="1:8" ht="12.75">
-      <c r="A113" s="7"/>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="9"/>
-      <c r="E113" s="17"/>
-      <c r="F113" s="9"/>
-      <c r="G113" s="13"/>
-      <c r="H113" s="13"/>
-    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B85:D85"/>
+  <mergeCells count="12">
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B84:D84"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D10:D12 F10:F12 H10:H12 D14:D16 F14:F16 H14:H16 D18:D21 F18:F21 H18:H21 D23 F23 H23 D25:D26 F25:F26 D28:D29 F28:F29 D31:D38 F31:F38 D40:D46 F40:F46 D48:D51 F48:F51 D53:D57 F53:F57 D59:D63 F59:F63 D65:D73 F65:F73 D75:D84 F75:F84 D86:D91 F86:F91 D93:D95 F93:F113 D97:D113">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Pass">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D17:D20 F17:F20 H17:H20 D22 F22 H22 D24:D25 F24:F25 D27:D28 F27:F28 D30:D37 F30:F37 D39:D45 F39:F45 D47:D50 F47:F50 D52:D56 F52:F56 D58:D62 F58:F62 D64:D72 F64:F72 D74:D83 F74:F83 D85:D90 F85:F90 D92:D94 F92:F112 D96:D112 D15 F15 H15">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D10:D12 F10:F12 H10:H12 D14:D16 F14:F16 H14:H16 D18:D21 F18:F21 H18:H21 D23 F23 H23 D25:D26 F25:F26 D28:D29 F28:F29 D31:D38 F31:F38 D40:D46 F40:F46 D48:D51 F48:F51 D53:D57 F53:F57 D59:D63 F59:F63 D65:D73 F65:F73 D75:D84 F75:F84 D86:D91 F86:F91 D93:D95 F93:F113 D97:D113">
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D17:D20 F17:F20 H17:H20 D22 F22 H22 D24:D25 F24:F25 D27:D28 F27:F28 D30:D37 F30:F37 D39:D45 F39:F45 D47:D50 F47:F50 D52:D56 F52:F56 D58:D62 F58:F62 D64:D72 F64:F72 D74:D83 F74:F83 D85:D90 F85:F90 D92:D94 F92:F112 D96:D112 D15 F15 H15">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D10:D12 F10:F12 H10:H12 D14:D16 F14:F16 H14:H16 D18:D21 F18:F21 H18:H21 D23 F23 H23 D25:D26 F25:F26 D28:D29 F28:F29 D31:D38 F31:F38 D40:D46 F40:F46 D48:D51 F48:F51 D53:D57 F53:F57 D59:D63 F59:F63 D65:D73 F65:F73 D75:D84 F75:F84 D86:D91 F86:F91 D93:D95 F93:F113 D97:D113">
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Block / Skip">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D17:D20 F17:F20 H17:H20 D22 F22 H22 D24:D25 F24:F25 D27:D28 F27:F28 D30:D37 F30:F37 D39:D45 F39:F45 D47:D50 F47:F50 D52:D56 F52:F56 D58:D62 F58:F62 D64:D72 F64:F72 D74:D83 F74:F83 D85:D90 F85:F90 D92:D94 F92:F112 D96:D112 D15 F15 H15">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D8 F4:F8 H4:H8 D10:D12 F10:F12 H10:H12 D14:D16 F14:F16 H14:H16 D18:D21 F18:F21 H18:H21 D23 F23 H23 D25:D26 F25:F26 D28:D29 F28:F29 D31:D38 F31:F38 D40:D46 F40:F46 D48:D51 F48:F51 D53:D57 F53:F57 D59:D63 F59:F63 D65:D73 F65:F73 D75:D84 F75:F84 D86:D91 F86:F91 D93:D95 F93:F95 D97:D113 F97:F113" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D8 F4:F8 H4:H8 F92:F94 D96:D112 F96:F112 D17:D20 F17:F20 H17:H20 D22 F22 H22 D24:D25 F24:F25 D27:D28 F27:F28 D30:D37 F30:F37 D39:D45 F39:F45 D47:D50 F47:F50 D52:D56 F52:F56 D58:D62 F58:F62 D64:D72 F64:F72 D74:D83 F74:F83 D85:D90 F85:F90 D92:D94 H10:H15 F10:F15 D10:D15" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2630,9 +2575,9 @@
       <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="15"/>
       <c r="F7" s="6"/>
     </row>
@@ -2682,9 +2627,9 @@
       <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="15"/>
       <c r="F11" s="6"/>
     </row>
@@ -2734,9 +2679,9 @@
       <c r="A15" s="5">
         <v>4</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="15"/>
       <c r="F15" s="6"/>
     </row>
@@ -2786,9 +2731,9 @@
       <c r="A19" s="5">
         <v>5</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
       <c r="E19" s="15"/>
       <c r="F19" s="6"/>
     </row>
@@ -2838,9 +2783,9 @@
       <c r="A23" s="5">
         <v>6</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
       <c r="E23" s="15"/>
       <c r="F23" s="6"/>
     </row>
@@ -2890,9 +2835,9 @@
       <c r="A27" s="5">
         <v>7</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
       <c r="E27" s="15"/>
       <c r="F27" s="6"/>
     </row>
@@ -2914,9 +2859,9 @@
       <c r="A29" s="5">
         <v>8</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
       <c r="E29" s="20"/>
       <c r="F29" s="6"/>
     </row>
@@ -2952,9 +2897,9 @@
       <c r="A32" s="5">
         <v>9</v>
       </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
       <c r="E32" s="15"/>
       <c r="F32" s="6"/>
     </row>
@@ -3018,9 +2963,9 @@
       <c r="A37" s="5">
         <v>10</v>
       </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="15"/>
       <c r="F37" s="6"/>
     </row>
@@ -3084,9 +3029,9 @@
       <c r="A42" s="5">
         <v>11</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
       <c r="E42" s="15"/>
       <c r="F42" s="6"/>
     </row>
@@ -3326,9 +3271,9 @@
       <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -3382,9 +3327,9 @@
       <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -3438,9 +3383,9 @@
       <c r="A15" s="5">
         <v>4</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -3533,9 +3478,9 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -3560,9 +3505,9 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -3667,9 +3612,9 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -3739,9 +3684,9 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -3784,9 +3729,9 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -3838,9 +3783,9 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -3892,9 +3837,9 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="5"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
@@ -3982,9 +3927,9 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="5"/>
-      <c r="B72" s="37"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -4081,9 +4026,9 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="5"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="38"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
@@ -4144,9 +4089,9 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="5"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="38"/>
-      <c r="D90" s="38"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="39"/>
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -4180,9 +4125,9 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="5"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
       <c r="E94" s="15"/>
       <c r="F94" s="6"/>
       <c r="G94" s="13"/>
@@ -4496,9 +4441,9 @@
       <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -4552,9 +4497,9 @@
       <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -4608,9 +4553,9 @@
       <c r="A15" s="5">
         <v>4</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -4703,9 +4648,9 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -4730,9 +4675,9 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -4837,9 +4782,9 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -4909,9 +4854,9 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -4954,9 +4899,9 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -5008,9 +4953,9 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -5062,9 +5007,9 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="5"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
@@ -5152,9 +5097,9 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="5"/>
-      <c r="B72" s="37"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -5251,9 +5196,9 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="5"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="38"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
@@ -5314,9 +5259,9 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="5"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="38"/>
-      <c r="D90" s="38"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="39"/>
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -5350,9 +5295,9 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="5"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
       <c r="E94" s="15"/>
       <c r="F94" s="6"/>
       <c r="G94" s="13"/>

</xml_diff>

<commit_message>
register using valid Facebook user
</commit_message>
<xml_diff>
--- a/Manual Testing.xlsx
+++ b/Manual Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\sqa projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D6F63B-9AB1-49BB-AD60-4861D4911552}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18E6BF3-93B1-4FEC-8641-D15BCAD59B50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="135" windowWidth="13455" windowHeight="9675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="81">
   <si>
     <t>Project Name</t>
   </si>
@@ -250,9 +250,6 @@
     <t>2.5</t>
   </si>
   <si>
-    <t>2.7</t>
-  </si>
-  <si>
     <t>click on the project owner radio buttton</t>
   </si>
   <si>
@@ -266,6 +263,24 @@
   </si>
   <si>
     <t>The placeholder is removed and email  entered successfully and password is encrypted (***)</t>
+  </si>
+  <si>
+    <t>Register using valid facebook  user (who has an email)</t>
+  </si>
+  <si>
+    <t>click on Facebook icon</t>
+  </si>
+  <si>
+    <t>login to facebook when redirected to it</t>
+  </si>
+  <si>
+    <t>user is redirected to facebook  to register using it</t>
+  </si>
+  <si>
+    <t>user is returned to the application
+* sign-up is successful
+user is directed to home page
+* A verification mail is sent to the user</t>
   </si>
 </sst>
 </file>
@@ -435,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -497,12 +512,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -548,7 +557,79 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -997,89 +1078,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="37"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="A1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="65.25" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="56.25" customHeight="1">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="55.5" customHeight="1">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:10" ht="71.25" customHeight="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:10" ht="57" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="J6" s="23"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1101,10 +1182,10 @@
     <tabColor rgb="FFF1C232"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1148,7 +1229,7 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="4"/>
@@ -1162,7 +1243,7 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="6"/>
@@ -1176,10 +1257,10 @@
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="29" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -1198,7 +1279,7 @@
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1220,7 +1301,7 @@
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -1239,14 +1320,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="29" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="13"/>
@@ -1255,13 +1336,13 @@
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="29" t="s">
         <v>62</v>
       </c>
       <c r="D8" s="9"/>
@@ -1270,29 +1351,29 @@
       <c r="G8" s="13"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" s="34" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:8" s="32" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="5">
         <v>2</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-    </row>
-    <row r="10" spans="1:8" s="34" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="41" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" s="32" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>73</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>15</v>
@@ -1306,12 +1387,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="34" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A11" s="41" t="s">
+    <row r="11" spans="1:8" s="32" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A11" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>74</v>
+      <c r="B11" s="29" t="s">
+        <v>73</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>64</v>
@@ -1328,11 +1409,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="34" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A12" s="41" t="s">
+    <row r="12" spans="1:8" s="32" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A12" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="29" t="s">
         <v>57</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -1350,15 +1431,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="34" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:8" s="32" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A13" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="29" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="13"/>
@@ -1366,14 +1447,14 @@
       <c r="G13" s="13"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" s="34" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A14" s="41" t="s">
+    <row r="14" spans="1:8" s="32" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A14" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>62</v>
       </c>
       <c r="D14" s="9"/>
@@ -1382,42 +1463,52 @@
       <c r="G14" s="13"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A15" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A16" s="5">
-        <v>4</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="8"/>
+    <row r="15" spans="1:8" s="32" customFormat="1" ht="42" customHeight="1">
+      <c r="A15" s="5">
+        <v>3</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+    </row>
+    <row r="16" spans="1:8" s="32" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="32" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A17" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="D17" s="9" t="s">
         <v>16</v>
       </c>
@@ -1430,134 +1521,100 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="12"/>
+    <row r="18" spans="1:8" s="32" customFormat="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="19" spans="1:8" s="32" customFormat="1" ht="12.75">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="D19" s="9"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="F19" s="9"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" s="32" customFormat="1" ht="12.75">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="5">
-        <v>5</v>
-      </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="A21" s="5"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="12.75">
+      <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="5"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="1:8" ht="12.75">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" ht="12.75">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" ht="12.75">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="5"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8" ht="12.75">
+      <c r="A26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" ht="12.75">
       <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
       <c r="F27" s="9"/>
@@ -1566,28 +1623,28 @@
     </row>
     <row r="28" spans="1:8" ht="12.75">
       <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="9"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+    <row r="29" spans="1:8" ht="12.75">
+      <c r="A29" s="7"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" ht="12.75">
       <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
       <c r="F30" s="9"/>
@@ -1609,25 +1666,24 @@
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="9"/>
-      <c r="E32" s="10"/>
       <c r="F32" s="9"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" ht="12.75">
-      <c r="A33" s="7"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
+    <row r="33" spans="1:8">
+      <c r="A33" s="5"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" ht="12.75">
       <c r="A34" s="7"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
       <c r="F34" s="9"/>
@@ -1637,7 +1693,7 @@
     <row r="35" spans="1:8" ht="12.75">
       <c r="A35" s="7"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="10"/>
       <c r="F35" s="9"/>
@@ -1659,24 +1715,25 @@
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="9"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="5"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
+    <row r="38" spans="1:8" ht="12.75">
+      <c r="A38" s="7"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" ht="12.75">
       <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
       <c r="F39" s="9"/>
@@ -1686,27 +1743,27 @@
     <row r="40" spans="1:8" ht="12.75">
       <c r="A40" s="7"/>
       <c r="B40" s="11"/>
-      <c r="C40" s="8"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
       <c r="F40" s="9"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" ht="12.75">
-      <c r="A41" s="7"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
+    <row r="41" spans="1:8">
+      <c r="A41" s="5"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" ht="12.75">
       <c r="A42" s="7"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
       <c r="F42" s="9"/>
@@ -1736,18 +1793,18 @@
     <row r="45" spans="1:8" ht="12.75">
       <c r="A45" s="7"/>
       <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
+      <c r="C45" s="8"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="10"/>
+      <c r="E45" s="13"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="5"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -1766,7 +1823,7 @@
     <row r="48" spans="1:8" ht="12.75">
       <c r="A48" s="7"/>
       <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
+      <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="10"/>
       <c r="F48" s="9"/>
@@ -1776,7 +1833,7 @@
     <row r="49" spans="1:8" ht="12.75">
       <c r="A49" s="7"/>
       <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
+      <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
       <c r="F49" s="9"/>
@@ -1786,36 +1843,36 @@
     <row r="50" spans="1:8" ht="12.75">
       <c r="A50" s="7"/>
       <c r="B50" s="11"/>
-      <c r="C50" s="8"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="9"/>
-      <c r="E50" s="13"/>
+      <c r="E50" s="10"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="5"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-    </row>
-    <row r="52" spans="1:8" ht="12.75">
-      <c r="A52" s="7"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+    </row>
+    <row r="51" spans="1:8" ht="12.75">
+      <c r="A51" s="7"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="5"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" ht="12.75">
       <c r="A53" s="7"/>
-      <c r="B53" s="11"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
@@ -1836,7 +1893,7 @@
     <row r="55" spans="1:8" ht="12.75">
       <c r="A55" s="7"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
+      <c r="C55" s="8"/>
       <c r="D55" s="9"/>
       <c r="E55" s="10"/>
       <c r="F55" s="9"/>
@@ -1846,36 +1903,36 @@
     <row r="56" spans="1:8" ht="12.75">
       <c r="A56" s="7"/>
       <c r="B56" s="11"/>
-      <c r="C56" s="8"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="13"/>
+      <c r="E56" s="10"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="5"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-    </row>
-    <row r="58" spans="1:8" ht="12.75">
-      <c r="A58" s="7"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="1:8" ht="12.75">
+      <c r="A57" s="7"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="5"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
     </row>
     <row r="59" spans="1:8" ht="12.75">
       <c r="A59" s="7"/>
-      <c r="B59" s="11"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="9"/>
       <c r="E59" s="10"/>
@@ -1896,7 +1953,7 @@
     <row r="61" spans="1:8" ht="12.75">
       <c r="A61" s="7"/>
       <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
+      <c r="C61" s="8"/>
       <c r="D61" s="9"/>
       <c r="E61" s="10"/>
       <c r="F61" s="9"/>
@@ -1906,47 +1963,47 @@
     <row r="62" spans="1:8" ht="12.75">
       <c r="A62" s="7"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="8"/>
+      <c r="C62" s="11"/>
       <c r="D62" s="9"/>
-      <c r="E62" s="13"/>
+      <c r="E62" s="10"/>
       <c r="F62" s="9"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="5"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
-      <c r="H63" s="6"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:8" ht="12.75">
+      <c r="A63" s="7"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" ht="12.75">
       <c r="A64" s="7"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="9"/>
-      <c r="E64" s="10"/>
+      <c r="E64" s="13"/>
       <c r="F64" s="9"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="12.75">
       <c r="A65" s="7"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="8"/>
+      <c r="C65" s="11"/>
       <c r="D65" s="9"/>
-      <c r="E65" s="10"/>
+      <c r="E65" s="13"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="10"/>
-      <c r="H65" s="10"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="12.75">
       <c r="A66" s="7"/>
       <c r="B66" s="11"/>
-      <c r="C66" s="8"/>
+      <c r="C66" s="11"/>
       <c r="D66" s="9"/>
       <c r="E66" s="10"/>
       <c r="F66" s="9"/>
@@ -1963,40 +2020,40 @@
       <c r="G67" s="10"/>
       <c r="H67" s="10"/>
     </row>
-    <row r="68" spans="1:8" ht="12.75">
-      <c r="A68" s="7"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="10"/>
-      <c r="H68" s="10"/>
+    <row r="68" spans="1:8">
+      <c r="A68" s="5"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
     </row>
     <row r="69" spans="1:8" ht="12.75">
       <c r="A69" s="7"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
       <c r="D69" s="9"/>
-      <c r="E69" s="13"/>
+      <c r="E69" s="10"/>
       <c r="F69" s="9"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="12.75">
       <c r="A70" s="7"/>
       <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
+      <c r="C70" s="8"/>
       <c r="D70" s="9"/>
-      <c r="E70" s="13"/>
+      <c r="E70" s="10"/>
       <c r="F70" s="9"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
     </row>
     <row r="71" spans="1:8" ht="12.75">
       <c r="A71" s="7"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
+      <c r="C71" s="8"/>
       <c r="D71" s="9"/>
       <c r="E71" s="10"/>
       <c r="F71" s="9"/>
@@ -2013,30 +2070,30 @@
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="5"/>
-      <c r="B73" s="38"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
+    <row r="73" spans="1:8" ht="12.75">
+      <c r="A73" s="7"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
     </row>
     <row r="74" spans="1:8" ht="12.75">
       <c r="A74" s="7"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="9"/>
-      <c r="E74" s="10"/>
+      <c r="E74" s="13"/>
       <c r="F74" s="9"/>
-      <c r="G74" s="10"/>
-      <c r="H74" s="10"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
     </row>
     <row r="75" spans="1:8" ht="12.75">
       <c r="A75" s="7"/>
       <c r="B75" s="11"/>
-      <c r="C75" s="8"/>
+      <c r="C75" s="11"/>
       <c r="D75" s="9"/>
       <c r="E75" s="10"/>
       <c r="F75" s="9"/>
@@ -2046,7 +2103,7 @@
     <row r="76" spans="1:8" ht="12.75">
       <c r="A76" s="7"/>
       <c r="B76" s="11"/>
-      <c r="C76" s="8"/>
+      <c r="C76" s="11"/>
       <c r="D76" s="9"/>
       <c r="E76" s="10"/>
       <c r="F76" s="9"/>
@@ -2073,20 +2130,20 @@
       <c r="G78" s="10"/>
       <c r="H78" s="10"/>
     </row>
-    <row r="79" spans="1:8" ht="12.75">
-      <c r="A79" s="7"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
+    <row r="79" spans="1:8">
+      <c r="A79" s="5"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
     </row>
     <row r="80" spans="1:8" ht="12.75">
       <c r="A80" s="7"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="11"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
       <c r="D80" s="9"/>
       <c r="E80" s="10"/>
       <c r="F80" s="9"/>
@@ -2123,40 +2180,40 @@
       <c r="G83" s="10"/>
       <c r="H83" s="10"/>
     </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="5"/>
-      <c r="B84" s="38"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
-      <c r="H84" s="6"/>
+    <row r="84" spans="1:8" ht="12.75">
+      <c r="A84" s="7"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
     </row>
     <row r="85" spans="1:8" ht="12.75">
       <c r="A85" s="7"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
       <c r="D85" s="9"/>
       <c r="E85" s="10"/>
       <c r="F85" s="9"/>
       <c r="G85" s="10"/>
       <c r="H85" s="10"/>
     </row>
-    <row r="86" spans="1:8" ht="12.75">
-      <c r="A86" s="7"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="11"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="10"/>
-      <c r="H86" s="10"/>
+    <row r="86" spans="1:8">
+      <c r="A86" s="5"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
     </row>
     <row r="87" spans="1:8" ht="12.75">
       <c r="A87" s="7"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="11"/>
+      <c r="B87" s="12"/>
+      <c r="C87" s="8"/>
       <c r="D87" s="9"/>
       <c r="E87" s="10"/>
       <c r="F87" s="9"/>
@@ -2165,8 +2222,8 @@
     </row>
     <row r="88" spans="1:8" ht="12.75">
       <c r="A88" s="7"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="8"/>
       <c r="D88" s="9"/>
       <c r="E88" s="10"/>
       <c r="F88" s="9"/>
@@ -2175,78 +2232,78 @@
     </row>
     <row r="89" spans="1:8" ht="12.75">
       <c r="A89" s="7"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
+      <c r="B89" s="12"/>
+      <c r="C89" s="8"/>
       <c r="D89" s="9"/>
       <c r="E89" s="10"/>
       <c r="F89" s="9"/>
-      <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
-    </row>
-    <row r="90" spans="1:8" ht="12.75">
-      <c r="A90" s="7"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="9"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="9"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="5"/>
-      <c r="B91" s="38"/>
-      <c r="C91" s="39"/>
-      <c r="D91" s="39"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="6"/>
-      <c r="H91" s="6"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="5"/>
+      <c r="B90" s="36"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+    </row>
+    <row r="91" spans="1:8" ht="12.75">
+      <c r="A91" s="7"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="16"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
     </row>
     <row r="92" spans="1:8" ht="12.75">
       <c r="A92" s="7"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="8"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
       <c r="D92" s="9"/>
-      <c r="E92" s="10"/>
+      <c r="E92" s="16"/>
       <c r="F92" s="9"/>
-      <c r="G92" s="10"/>
-      <c r="H92" s="10"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
     </row>
     <row r="93" spans="1:8" ht="12.75">
       <c r="A93" s="7"/>
-      <c r="B93" s="12"/>
-      <c r="C93" s="8"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="11"/>
       <c r="D93" s="9"/>
-      <c r="E93" s="10"/>
+      <c r="E93" s="16"/>
       <c r="F93" s="9"/>
-      <c r="G93" s="10"/>
-      <c r="H93" s="10"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
     </row>
     <row r="94" spans="1:8" ht="12.75">
       <c r="A94" s="7"/>
-      <c r="B94" s="12"/>
-      <c r="C94" s="8"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
       <c r="D94" s="9"/>
-      <c r="E94" s="10"/>
+      <c r="E94" s="16"/>
       <c r="F94" s="9"/>
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
     </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="5"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="15"/>
-      <c r="F95" s="6"/>
+    <row r="95" spans="1:8" ht="12.75">
+      <c r="A95" s="7"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="16"/>
+      <c r="F95" s="9"/>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
     </row>
     <row r="96" spans="1:8" ht="12.75">
       <c r="A96" s="7"/>
-      <c r="B96" s="8"/>
-      <c r="C96" s="8"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="11"/>
       <c r="D96" s="9"/>
       <c r="E96" s="16"/>
       <c r="F96" s="9"/>
@@ -2276,7 +2333,7 @@
     <row r="99" spans="1:8" ht="12.75">
       <c r="A99" s="7"/>
       <c r="B99" s="11"/>
-      <c r="C99" s="11"/>
+      <c r="C99" s="8"/>
       <c r="D99" s="9"/>
       <c r="E99" s="16"/>
       <c r="F99" s="9"/>
@@ -2286,7 +2343,7 @@
     <row r="100" spans="1:8" ht="12.75">
       <c r="A100" s="7"/>
       <c r="B100" s="11"/>
-      <c r="C100" s="8"/>
+      <c r="C100" s="11"/>
       <c r="D100" s="9"/>
       <c r="E100" s="16"/>
       <c r="F100" s="9"/>
@@ -2318,7 +2375,7 @@
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
       <c r="D103" s="9"/>
-      <c r="E103" s="16"/>
+      <c r="E103" s="17"/>
       <c r="F103" s="9"/>
       <c r="G103" s="13"/>
       <c r="H103" s="13"/>
@@ -2326,7 +2383,7 @@
     <row r="104" spans="1:8" ht="12.75">
       <c r="A104" s="7"/>
       <c r="B104" s="11"/>
-      <c r="C104" s="8"/>
+      <c r="C104" s="11"/>
       <c r="D104" s="9"/>
       <c r="E104" s="16"/>
       <c r="F104" s="9"/>
@@ -2338,7 +2395,7 @@
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
       <c r="D105" s="9"/>
-      <c r="E105" s="16"/>
+      <c r="E105" s="17"/>
       <c r="F105" s="9"/>
       <c r="G105" s="13"/>
       <c r="H105" s="13"/>
@@ -2358,108 +2415,72 @@
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
       <c r="D107" s="9"/>
-      <c r="E107" s="16"/>
+      <c r="E107" s="17"/>
       <c r="F107" s="9"/>
       <c r="G107" s="13"/>
       <c r="H107" s="13"/>
     </row>
-    <row r="108" spans="1:8" ht="12.75">
-      <c r="A108" s="7"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="17"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-    </row>
-    <row r="109" spans="1:8" ht="12.75">
-      <c r="A109" s="7"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="9"/>
-      <c r="E109" s="16"/>
-      <c r="F109" s="9"/>
-      <c r="G109" s="13"/>
-      <c r="H109" s="13"/>
-    </row>
-    <row r="110" spans="1:8" ht="12.75">
-      <c r="A110" s="7"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="9"/>
-      <c r="E110" s="17"/>
-      <c r="F110" s="9"/>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13"/>
-    </row>
-    <row r="111" spans="1:8" ht="12.75">
-      <c r="A111" s="7"/>
-      <c r="B111" s="11"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="9"/>
-      <c r="E111" s="16"/>
-      <c r="F111" s="9"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
-    </row>
-    <row r="112" spans="1:8" ht="12.75">
-      <c r="A112" s="7"/>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="9"/>
-      <c r="E112" s="17"/>
-      <c r="F112" s="9"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
-    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B38:D38"/>
+  <mergeCells count="11">
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B41:D41"/>
     <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B79:D79"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D17:D20 F17:F20 H17:H20 D22 F22 H22 D24:D25 F24:F25 D27:D28 F27:F28 D30:D37 F30:F37 D39:D45 F39:F45 D47:D50 F47:F50 D52:D56 F52:F56 D58:D62 F58:F62 D64:D72 F64:F72 D74:D83 F74:F83 D85:D90 F85:F90 D92:D94 F92:F112 D96:D112 D15 F15 H15">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Pass">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D19:D20 F19:F20 D22:D23 F22:F23 D25:D32 F25:F32 D34:D40 F34:F40 D42:D45 F42:F45 D47:D51 F47:F51 D53:D57 F53:F57 D59:D67 F59:F67 D69:D78 F69:F78 D80:D85 F80:F85 D87:D89 F87:F107 D91:D107">
+    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D17:D20 F17:F20 H17:H20 D22 F22 H22 D24:D25 F24:F25 D27:D28 F27:F28 D30:D37 F30:F37 D39:D45 F39:F45 D47:D50 F47:F50 D52:D56 F52:F56 D58:D62 F58:F62 D64:D72 F64:F72 D74:D83 F74:F83 D85:D90 F85:F90 D92:D94 F92:F112 D96:D112 D15 F15 H15">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D19:D20 F19:F20 D22:D23 F22:F23 D25:D32 F25:F32 D34:D40 F34:F40 D42:D45 F42:F45 D47:D51 F47:F51 D53:D57 F53:F57 D59:D67 F59:F67 D69:D78 F69:F78 D80:D85 F80:F85 D87:D89 F87:F107 D91:D107">
+    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D17:D20 F17:F20 H17:H20 D22 F22 H22 D24:D25 F24:F25 D27:D28 F27:F28 D30:D37 F30:F37 D39:D45 F39:F45 D47:D50 F47:F50 D52:D56 F52:F56 D58:D62 F58:F62 D64:D72 F64:F72 D74:D83 F74:F83 D85:D90 F85:F90 D92:D94 F92:F112 D96:D112 D15 F15 H15">
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Block / Skip">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D19:D20 F19:F20 D22:D23 F22:F23 D25:D32 F25:F32 D34:D40 F34:F40 D42:D45 F42:F45 D47:D51 F47:F51 D53:D57 F53:F57 D59:D67 F59:F67 D69:D78 F69:F78 D80:D85 F80:F85 D87:D89 F87:F107 D91:D107">
+    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D8 F4:F8 H4:H8 F92:F94 D96:D112 F96:F112 D17:D20 F17:F20 H17:H20 D22 F22 H22 D24:D25 F24:F25 D27:D28 F27:F28 D30:D37 F30:F37 D39:D45 F39:F45 D47:D50 F47:F50 D52:D56 F52:F56 D58:D62 F58:F62 D64:D72 F64:F72 D74:D83 F74:F83 D85:D90 F85:F90 D92:D94 H10:H15 F10:F15 D10:D15" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D8 F4:F8 H4:H8 F87:F89 D91:D107 F91:F107 D80:D85 F80:F85 D87:D89 H10:H14 F10:F14 D10:D14 D19:D20 F19:F20 D22:D23 F22:F23 D25:D32 F25:F32 D34:D40 F34:F40 D42:D45 F42:F45 D47:D51 F47:F51 D53:D57 F53:F57 D59:D67 F59:F67 D69:D78 F69:F78 D16:D17 F16:F17 H16:H17" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2575,9 +2596,9 @@
       <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="15"/>
       <c r="F7" s="6"/>
     </row>
@@ -2627,9 +2648,9 @@
       <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="15"/>
       <c r="F11" s="6"/>
     </row>
@@ -2679,9 +2700,9 @@
       <c r="A15" s="5">
         <v>4</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="15"/>
       <c r="F15" s="6"/>
     </row>
@@ -2731,9 +2752,9 @@
       <c r="A19" s="5">
         <v>5</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="15"/>
       <c r="F19" s="6"/>
     </row>
@@ -2783,9 +2804,9 @@
       <c r="A23" s="5">
         <v>6</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="15"/>
       <c r="F23" s="6"/>
     </row>
@@ -2835,9 +2856,9 @@
       <c r="A27" s="5">
         <v>7</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="15"/>
       <c r="F27" s="6"/>
     </row>
@@ -2859,9 +2880,9 @@
       <c r="A29" s="5">
         <v>8</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="20"/>
       <c r="F29" s="6"/>
     </row>
@@ -2897,9 +2918,9 @@
       <c r="A32" s="5">
         <v>9</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="15"/>
       <c r="F32" s="6"/>
     </row>
@@ -2963,9 +2984,9 @@
       <c r="A37" s="5">
         <v>10</v>
       </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="15"/>
       <c r="F37" s="6"/>
     </row>
@@ -3029,9 +3050,9 @@
       <c r="A42" s="5">
         <v>11</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
       <c r="E42" s="15"/>
       <c r="F42" s="6"/>
     </row>
@@ -3271,9 +3292,9 @@
       <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -3327,9 +3348,9 @@
       <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -3383,9 +3404,9 @@
       <c r="A15" s="5">
         <v>4</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -3478,9 +3499,9 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -3505,9 +3526,9 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -3612,9 +3633,9 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -3684,9 +3705,9 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -3729,9 +3750,9 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -3783,9 +3804,9 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -3837,9 +3858,9 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="5"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
@@ -3927,9 +3948,9 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="5"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -4026,9 +4047,9 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="5"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="37"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
@@ -4089,9 +4110,9 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="5"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
+      <c r="B90" s="36"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -4125,9 +4146,9 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="5"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
       <c r="E94" s="15"/>
       <c r="F94" s="6"/>
       <c r="G94" s="13"/>
@@ -4441,9 +4462,9 @@
       <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -4497,9 +4518,9 @@
       <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -4553,9 +4574,9 @@
       <c r="A15" s="5">
         <v>4</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -4648,9 +4669,9 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -4675,9 +4696,9 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -4782,9 +4803,9 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -4854,9 +4875,9 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -4899,9 +4920,9 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -4953,9 +4974,9 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -5007,9 +5028,9 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="5"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
@@ -5097,9 +5118,9 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="5"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -5196,9 +5217,9 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="5"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="37"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
@@ -5259,9 +5280,9 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="5"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
+      <c r="B90" s="36"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -5295,9 +5316,9 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="5"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
       <c r="E94" s="15"/>
       <c r="F94" s="6"/>
       <c r="G94" s="13"/>

</xml_diff>

<commit_message>
register using valid FB user who registered using phone or email
</commit_message>
<xml_diff>
--- a/Manual Testing.xlsx
+++ b/Manual Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\sqa projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18E6BF3-93B1-4FEC-8641-D15BCAD59B50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA84924B-B6C7-40B2-B7DF-F3A41E9DE301}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6420" yWindow="135" windowWidth="13455" windowHeight="9675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="89">
   <si>
     <t>Project Name</t>
   </si>
@@ -281,6 +281,34 @@
 * sign-up is successful
 user is directed to home page
 * A verification mail is sent to the user</t>
+  </si>
+  <si>
+    <t>Register using valid facebook  user (who registered to facebook using a phone number)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user is returned to the application
+* user is asked to enter his email
+* </t>
+  </si>
+  <si>
+    <t>The placeholder is removed and email is entered successfully</t>
+  </si>
+  <si>
+    <t>The password Is encrypted (****)</t>
+  </si>
+  <si>
+    <t>Enter a valid password</t>
+  </si>
+  <si>
+    <t>Click on Sign-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Sign-up is successful
+* user is redirected to home page
+* A verification mail is sent to the user </t>
+  </si>
+  <si>
+    <t>4.5</t>
   </si>
 </sst>
 </file>
@@ -557,31 +585,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1182,10 +1186,10 @@
     <tabColor rgb="FFF1C232"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1521,71 +1525,117 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="32" customFormat="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+    <row r="18" spans="1:8" s="32" customFormat="1" ht="42" customHeight="1">
+      <c r="A18" s="5">
+        <v>4</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
     </row>
-    <row r="19" spans="1:8" s="32" customFormat="1" ht="12.75">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+    <row r="19" spans="1:8" s="32" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A19" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="E19" s="13"/>
-      <c r="F19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" s="32" customFormat="1" ht="12.75">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="32" customFormat="1" ht="59.25" customHeight="1">
+      <c r="A20" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E20" s="13"/>
-      <c r="F20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="5"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" ht="12.75">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="H20" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="32" customFormat="1" ht="36" customHeight="1">
+      <c r="A21" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" s="32" customFormat="1" ht="36" customHeight="1">
+      <c r="A22" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" ht="12.75">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" s="32" customFormat="1" ht="66" customHeight="1">
+      <c r="A23" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -1603,28 +1653,28 @@
     </row>
     <row r="26" spans="1:8" ht="12.75">
       <c r="A26" s="7"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
       <c r="F26" s="9"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8" ht="12.75">
-      <c r="A27" s="7"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+    <row r="27" spans="1:8">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" ht="12.75">
       <c r="A28" s="7"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="9"/>
@@ -1666,24 +1716,25 @@
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="9"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="5"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+    <row r="33" spans="1:8" ht="12.75">
+      <c r="A33" s="7"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" ht="12.75">
       <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
       <c r="F34" s="9"/>
@@ -1693,27 +1744,26 @@
     <row r="35" spans="1:8" ht="12.75">
       <c r="A35" s="7"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="8"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="10"/>
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8" ht="12.75">
-      <c r="A36" s="7"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
+    <row r="36" spans="1:8">
+      <c r="A36" s="5"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" spans="1:8" ht="12.75">
       <c r="A37" s="7"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
       <c r="F37" s="9"/>
@@ -1723,7 +1773,7 @@
     <row r="38" spans="1:8" ht="12.75">
       <c r="A38" s="7"/>
       <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
       <c r="F38" s="9"/>
@@ -1750,20 +1800,20 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="5"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
+    <row r="41" spans="1:8" ht="12.75">
+      <c r="A41" s="7"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" ht="12.75">
       <c r="A42" s="7"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
       <c r="F42" s="9"/>
@@ -1780,40 +1830,40 @@
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" ht="12.75">
-      <c r="A44" s="7"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
+    <row r="44" spans="1:8">
+      <c r="A44" s="5"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" spans="1:8" ht="12.75">
       <c r="A45" s="7"/>
-      <c r="B45" s="11"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="13"/>
+      <c r="E45" s="10"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="5"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+    </row>
+    <row r="46" spans="1:8" ht="12.75">
+      <c r="A46" s="7"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" ht="12.75">
       <c r="A47" s="7"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="9"/>
       <c r="E47" s="10"/>
       <c r="F47" s="9"/>
@@ -1825,25 +1875,25 @@
       <c r="B48" s="11"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="10"/>
+      <c r="E48" s="13"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-    </row>
-    <row r="49" spans="1:8" ht="12.75">
-      <c r="A49" s="7"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="5"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" spans="1:8" ht="12.75">
       <c r="A50" s="7"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
       <c r="F50" s="9"/>
@@ -1855,25 +1905,25 @@
       <c r="B51" s="11"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
-      <c r="E51" s="13"/>
+      <c r="E51" s="10"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="5"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:8" ht="12.75">
+      <c r="A52" s="7"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" ht="12.75">
       <c r="A53" s="7"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
       <c r="F53" s="9"/>
@@ -1885,25 +1935,25 @@
       <c r="B54" s="11"/>
       <c r="C54" s="8"/>
       <c r="D54" s="9"/>
-      <c r="E54" s="10"/>
+      <c r="E54" s="13"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-    </row>
-    <row r="55" spans="1:8" ht="12.75">
-      <c r="A55" s="7"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="5"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" ht="12.75">
       <c r="A56" s="7"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
       <c r="D56" s="9"/>
       <c r="E56" s="10"/>
       <c r="F56" s="9"/>
@@ -1915,25 +1965,25 @@
       <c r="B57" s="11"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
-      <c r="E57" s="13"/>
+      <c r="E57" s="10"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="5"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+    </row>
+    <row r="58" spans="1:8" ht="12.75">
+      <c r="A58" s="7"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" ht="12.75">
       <c r="A59" s="7"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
       <c r="D59" s="9"/>
       <c r="E59" s="10"/>
       <c r="F59" s="9"/>
@@ -1945,25 +1995,25 @@
       <c r="B60" s="11"/>
       <c r="C60" s="8"/>
       <c r="D60" s="9"/>
-      <c r="E60" s="10"/>
+      <c r="E60" s="13"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-    </row>
-    <row r="61" spans="1:8" ht="12.75">
-      <c r="A61" s="7"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="5"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8" ht="12.75">
       <c r="A62" s="7"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
       <c r="D62" s="9"/>
       <c r="E62" s="10"/>
       <c r="F62" s="9"/>
@@ -1973,7 +2023,7 @@
     <row r="63" spans="1:8" ht="12.75">
       <c r="A63" s="7"/>
       <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
+      <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="10"/>
       <c r="F63" s="9"/>
@@ -1983,22 +2033,22 @@
     <row r="64" spans="1:8" ht="12.75">
       <c r="A64" s="7"/>
       <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
+      <c r="C64" s="8"/>
       <c r="D64" s="9"/>
-      <c r="E64" s="13"/>
+      <c r="E64" s="10"/>
       <c r="F64" s="9"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" ht="12.75">
       <c r="A65" s="7"/>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
       <c r="D65" s="9"/>
-      <c r="E65" s="13"/>
+      <c r="E65" s="10"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" ht="12.75">
       <c r="A66" s="7"/>
@@ -2015,25 +2065,25 @@
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
       <c r="D67" s="9"/>
-      <c r="E67" s="10"/>
+      <c r="E67" s="13"/>
       <c r="F67" s="9"/>
-      <c r="G67" s="10"/>
-      <c r="H67" s="10"/>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="5"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+    </row>
+    <row r="68" spans="1:8" ht="12.75">
+      <c r="A68" s="7"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
     </row>
     <row r="69" spans="1:8" ht="12.75">
       <c r="A69" s="7"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
       <c r="D69" s="9"/>
       <c r="E69" s="10"/>
       <c r="F69" s="9"/>
@@ -2043,27 +2093,27 @@
     <row r="70" spans="1:8" ht="12.75">
       <c r="A70" s="7"/>
       <c r="B70" s="11"/>
-      <c r="C70" s="8"/>
+      <c r="C70" s="11"/>
       <c r="D70" s="9"/>
       <c r="E70" s="10"/>
       <c r="F70" s="9"/>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
     </row>
-    <row r="71" spans="1:8" ht="12.75">
-      <c r="A71" s="7"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
+    <row r="71" spans="1:8">
+      <c r="A71" s="5"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
     </row>
     <row r="72" spans="1:8" ht="12.75">
       <c r="A72" s="7"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
       <c r="D72" s="9"/>
       <c r="E72" s="10"/>
       <c r="F72" s="9"/>
@@ -2073,7 +2123,7 @@
     <row r="73" spans="1:8" ht="12.75">
       <c r="A73" s="7"/>
       <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
+      <c r="C73" s="8"/>
       <c r="D73" s="9"/>
       <c r="E73" s="10"/>
       <c r="F73" s="9"/>
@@ -2083,12 +2133,12 @@
     <row r="74" spans="1:8" ht="12.75">
       <c r="A74" s="7"/>
       <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
+      <c r="C74" s="8"/>
       <c r="D74" s="9"/>
-      <c r="E74" s="13"/>
+      <c r="E74" s="10"/>
       <c r="F74" s="9"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
     </row>
     <row r="75" spans="1:8" ht="12.75">
       <c r="A75" s="7"/>
@@ -2115,10 +2165,10 @@
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
       <c r="D77" s="9"/>
-      <c r="E77" s="10"/>
+      <c r="E77" s="13"/>
       <c r="F77" s="9"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="10"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
     </row>
     <row r="78" spans="1:8" ht="12.75">
       <c r="A78" s="7"/>
@@ -2130,20 +2180,20 @@
       <c r="G78" s="10"/>
       <c r="H78" s="10"/>
     </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="5"/>
-      <c r="B79" s="36"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
+    <row r="79" spans="1:8" ht="12.75">
+      <c r="A79" s="7"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
     </row>
     <row r="80" spans="1:8" ht="12.75">
       <c r="A80" s="7"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
       <c r="D80" s="9"/>
       <c r="E80" s="10"/>
       <c r="F80" s="9"/>
@@ -2160,20 +2210,20 @@
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
     </row>
-    <row r="82" spans="1:8" ht="12.75">
-      <c r="A82" s="7"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="10"/>
-      <c r="H82" s="10"/>
+    <row r="82" spans="1:8">
+      <c r="A82" s="5"/>
+      <c r="B82" s="36"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
     </row>
     <row r="83" spans="1:8" ht="12.75">
       <c r="A83" s="7"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="11"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
       <c r="D83" s="9"/>
       <c r="E83" s="10"/>
       <c r="F83" s="9"/>
@@ -2200,20 +2250,20 @@
       <c r="G85" s="10"/>
       <c r="H85" s="10"/>
     </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="5"/>
-      <c r="B86" s="36"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="6"/>
+    <row r="86" spans="1:8" ht="12.75">
+      <c r="A86" s="7"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
     </row>
     <row r="87" spans="1:8" ht="12.75">
       <c r="A87" s="7"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="8"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
       <c r="D87" s="9"/>
       <c r="E87" s="10"/>
       <c r="F87" s="9"/>
@@ -2222,68 +2272,68 @@
     </row>
     <row r="88" spans="1:8" ht="12.75">
       <c r="A88" s="7"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="8"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
       <c r="D88" s="9"/>
       <c r="E88" s="10"/>
       <c r="F88" s="9"/>
       <c r="G88" s="10"/>
       <c r="H88" s="10"/>
     </row>
-    <row r="89" spans="1:8" ht="12.75">
-      <c r="A89" s="7"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="9"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="5"/>
-      <c r="B90" s="36"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="6"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
+    <row r="89" spans="1:8">
+      <c r="A89" s="5"/>
+      <c r="B89" s="36"/>
+      <c r="C89" s="37"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+    </row>
+    <row r="90" spans="1:8" ht="12.75">
+      <c r="A90" s="7"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
     </row>
     <row r="91" spans="1:8" ht="12.75">
       <c r="A91" s="7"/>
-      <c r="B91" s="8"/>
+      <c r="B91" s="12"/>
       <c r="C91" s="8"/>
       <c r="D91" s="9"/>
-      <c r="E91" s="16"/>
+      <c r="E91" s="10"/>
       <c r="F91" s="9"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
     </row>
     <row r="92" spans="1:8" ht="12.75">
       <c r="A92" s="7"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="11"/>
+      <c r="B92" s="12"/>
+      <c r="C92" s="8"/>
       <c r="D92" s="9"/>
-      <c r="E92" s="16"/>
+      <c r="E92" s="10"/>
       <c r="F92" s="9"/>
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
     </row>
-    <row r="93" spans="1:8" ht="12.75">
-      <c r="A93" s="7"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="16"/>
-      <c r="F93" s="9"/>
+    <row r="93" spans="1:8">
+      <c r="A93" s="5"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="6"/>
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
     </row>
     <row r="94" spans="1:8" ht="12.75">
       <c r="A94" s="7"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
       <c r="D94" s="9"/>
       <c r="E94" s="16"/>
       <c r="F94" s="9"/>
@@ -2293,7 +2343,7 @@
     <row r="95" spans="1:8" ht="12.75">
       <c r="A95" s="7"/>
       <c r="B95" s="11"/>
-      <c r="C95" s="8"/>
+      <c r="C95" s="11"/>
       <c r="D95" s="9"/>
       <c r="E95" s="16"/>
       <c r="F95" s="9"/>
@@ -2323,7 +2373,7 @@
     <row r="98" spans="1:8" ht="12.75">
       <c r="A98" s="7"/>
       <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
+      <c r="C98" s="8"/>
       <c r="D98" s="9"/>
       <c r="E98" s="16"/>
       <c r="F98" s="9"/>
@@ -2333,7 +2383,7 @@
     <row r="99" spans="1:8" ht="12.75">
       <c r="A99" s="7"/>
       <c r="B99" s="11"/>
-      <c r="C99" s="8"/>
+      <c r="C99" s="11"/>
       <c r="D99" s="9"/>
       <c r="E99" s="16"/>
       <c r="F99" s="9"/>
@@ -2363,7 +2413,7 @@
     <row r="102" spans="1:8" ht="12.75">
       <c r="A102" s="7"/>
       <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
+      <c r="C102" s="8"/>
       <c r="D102" s="9"/>
       <c r="E102" s="16"/>
       <c r="F102" s="9"/>
@@ -2375,7 +2425,7 @@
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
       <c r="D103" s="9"/>
-      <c r="E103" s="17"/>
+      <c r="E103" s="16"/>
       <c r="F103" s="9"/>
       <c r="G103" s="13"/>
       <c r="H103" s="13"/>
@@ -2395,7 +2445,7 @@
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
       <c r="D105" s="9"/>
-      <c r="E105" s="17"/>
+      <c r="E105" s="16"/>
       <c r="F105" s="9"/>
       <c r="G105" s="13"/>
       <c r="H105" s="13"/>
@@ -2405,7 +2455,7 @@
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="9"/>
-      <c r="E106" s="16"/>
+      <c r="E106" s="17"/>
       <c r="F106" s="9"/>
       <c r="G106" s="13"/>
       <c r="H106" s="13"/>
@@ -2415,72 +2465,116 @@
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
       <c r="D107" s="9"/>
-      <c r="E107" s="17"/>
+      <c r="E107" s="16"/>
       <c r="F107" s="9"/>
       <c r="G107" s="13"/>
       <c r="H107" s="13"/>
     </row>
+    <row r="108" spans="1:8" ht="12.75">
+      <c r="A108" s="7"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+    </row>
+    <row r="109" spans="1:8" ht="12.75">
+      <c r="A109" s="7"/>
+      <c r="B109" s="11"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="16"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="13"/>
+      <c r="H109" s="13"/>
+    </row>
+    <row r="110" spans="1:8" ht="12.75">
+      <c r="A110" s="7"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="17"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B79:D79"/>
+  <mergeCells count="10">
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B82:D82"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D19:D20 F19:F20 D22:D23 F22:F23 D25:D32 F25:F32 D34:D40 F34:F40 D42:D45 F42:F45 D47:D51 F47:F51 D53:D57 F53:F57 D59:D67 F59:F67 D69:D78 F69:F78 D80:D85 F80:F85 D87:D89 F87:F107 D91:D107">
-    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="Pass">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D25:D26 F25:F26 D28:D35 F28:F35 D37:D43 F37:F43 D45:D48 F45:F48 D50:D54 F50:F54 D56:D60 F56:F60 D62:D70 F62:F70 D72:D81 F72:F81 D83:D88 F83:F88 D90:D92 F90:F110 D94:D110 D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D19:D20 F19:F20 D22:D23 F22:F23 D25:D32 F25:F32 D34:D40 F34:F40 D42:D45 F42:F45 D47:D51 F47:F51 D53:D57 F53:F57 D59:D67 F59:F67 D69:D78 F69:F78 D80:D85 F80:F85 D87:D89 F87:F107 D91:D107">
-    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D25:D26 F25:F26 D28:D35 F28:F35 D37:D43 F37:F43 D45:D48 F45:F48 D50:D54 F50:F54 D56:D60 F56:F60 D62:D70 F62:F70 D72:D81 F72:F81 D83:D88 F83:F88 D90:D92 F90:F110 D94:D110 D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D19:D20 F19:F20 D22:D23 F22:F23 D25:D32 F25:F32 D34:D40 F34:F40 D42:D45 F42:F45 D47:D51 F47:F51 D53:D57 F53:F57 D59:D67 F59:F67 D69:D78 F69:F78 D80:D85 F80:F85 D87:D89 F87:F107 D91:D107">
-    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="Block / Skip">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D25:D26 F25:F26 D28:D35 F28:F35 D37:D43 F37:F43 D45:D48 F45:F48 D50:D54 F50:F54 D56:D60 F56:F60 D62:D70 F62:F70 D72:D81 F72:F81 D83:D88 F83:F88 D90:D92 F90:F110 D94:D110 D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D17 F16:F17 H16:H17">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH(("Pass"),(D16))))</formula>
+  <conditionalFormatting sqref="D19:D20 F19:F20 H19:H20">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D19))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D17 F16:F17 H16:H17">
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH(("Fail"),(D16))))</formula>
+  <conditionalFormatting sqref="D19:D20 F19:F20 H19:H20">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D19))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D17 F16:F17 H16:H17">
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="Block / Skip">
-      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D16))))</formula>
+  <conditionalFormatting sqref="D19:D20 F19:F20 H19:H20">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D23 F21:F23 H21:H23">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D23 F21:F23 H21:H23">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D23 F21:F23 H21:H23">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D21))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D8 F4:F8 H4:H8 F87:F89 D91:D107 F91:F107 D80:D85 F80:F85 D87:D89 H10:H14 F10:F14 D10:D14 D19:D20 F19:F20 D22:D23 F22:F23 D25:D32 F25:F32 D34:D40 F34:F40 D42:D45 F42:F45 D47:D51 F47:F51 D53:D57 F53:F57 D59:D67 F59:F67 D69:D78 F69:F78 D16:D17 F16:F17 H16:H17" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D8 F4:F8 H4:H8 F90:F92 D94:D110 F94:F110 D83:D88 F83:F88 D90:D92 H10:H14 F10:F14 D10:D14 D25:D26 F25:F26 D28:D35 F28:F35 D37:D43 F37:F43 D45:D48 F45:F48 D50:D54 F50:F54 D56:D60 F56:F60 D62:D70 F62:F70 D72:D81 F72:F81 D19:D23 H19:H23 F19:F23 F16:F17 H16:H17 D16:D17" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
register using valid Gmail user
</commit_message>
<xml_diff>
--- a/Manual Testing.xlsx
+++ b/Manual Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\sqa projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA84924B-B6C7-40B2-B7DF-F3A41E9DE301}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CE5A0D-4C2E-482F-A877-DFAA5126F42B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="135" windowWidth="13455" windowHeight="9675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="95">
   <si>
     <t>Project Name</t>
   </si>
@@ -309,6 +309,27 @@
   </si>
   <si>
     <t>4.5</t>
+  </si>
+  <si>
+    <t>Register using valid gmail user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user is redirected to his gmail accounts page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose an account </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* user is redirected to application
+* registration is done successfully
+* user is redirected to homepage
+</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Block / Skip</t>
   </si>
 </sst>
 </file>
@@ -585,7 +606,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1186,10 +1231,10 @@
     <tabColor rgb="FFF1C232"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1333,7 +1378,9 @@
       <c r="C7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="E7" s="13"/>
       <c r="F7" s="9"/>
       <c r="G7" s="13"/>
@@ -1349,7 +1396,9 @@
       <c r="C8" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="E8" s="13"/>
       <c r="F8" s="9"/>
       <c r="G8" s="13"/>
@@ -1445,7 +1494,9 @@
       <c r="C13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="9"/>
       <c r="G13" s="13"/>
@@ -1461,7 +1512,9 @@
       <c r="C14" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E14" s="13"/>
       <c r="F14" s="9"/>
       <c r="G14" s="13"/>
@@ -1631,41 +1684,69 @@
       <c r="G23" s="13"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="5"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" ht="12.75">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:8" ht="12.75">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+    <row r="24" spans="1:8" s="32" customFormat="1" ht="42" customHeight="1">
+      <c r="A24" s="5">
+        <v>5</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="25" spans="1:8" s="32" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A25" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="32" customFormat="1" ht="59.25" customHeight="1">
+      <c r="A26" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -1684,7 +1765,7 @@
     <row r="29" spans="1:8" ht="12.75">
       <c r="A29" s="7"/>
       <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
       <c r="F29" s="9"/>
@@ -1741,29 +1822,30 @@
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="1:8" ht="12.75">
-      <c r="A35" s="7"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="5"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" ht="12.75">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" ht="12.75">
       <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
       <c r="F37" s="9"/>
@@ -1773,7 +1855,7 @@
     <row r="38" spans="1:8" ht="12.75">
       <c r="A38" s="7"/>
       <c r="B38" s="11"/>
-      <c r="C38" s="8"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
       <c r="F38" s="9"/>
@@ -1783,27 +1865,27 @@
     <row r="39" spans="1:8" ht="12.75">
       <c r="A39" s="7"/>
       <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="9"/>
-      <c r="E39" s="10"/>
+      <c r="E39" s="13"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-    </row>
-    <row r="40" spans="1:8" ht="12.75">
-      <c r="A40" s="7"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="5"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" ht="12.75">
       <c r="A41" s="7"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
       <c r="F41" s="9"/>
@@ -1813,7 +1895,7 @@
     <row r="42" spans="1:8" ht="12.75">
       <c r="A42" s="7"/>
       <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+      <c r="C42" s="8"/>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
       <c r="F42" s="9"/>
@@ -1823,47 +1905,47 @@
     <row r="43" spans="1:8" ht="12.75">
       <c r="A43" s="7"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+      <c r="C43" s="8"/>
       <c r="D43" s="9"/>
       <c r="E43" s="10"/>
       <c r="F43" s="9"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="5"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
+    <row r="44" spans="1:8" ht="12.75">
+      <c r="A44" s="7"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" ht="12.75">
       <c r="A45" s="7"/>
-      <c r="B45" s="8"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="10"/>
+      <c r="E45" s="13"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-    </row>
-    <row r="46" spans="1:8" ht="12.75">
-      <c r="A46" s="7"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="5"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" ht="12.75">
       <c r="A47" s="7"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="10"/>
       <c r="F47" s="9"/>
@@ -1875,25 +1957,25 @@
       <c r="B48" s="11"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="13"/>
+      <c r="E48" s="10"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="5"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+    </row>
+    <row r="49" spans="1:8" ht="12.75">
+      <c r="A49" s="7"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" ht="12.75">
       <c r="A50" s="7"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
       <c r="F50" s="9"/>
@@ -1905,25 +1987,25 @@
       <c r="B51" s="11"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-    </row>
-    <row r="52" spans="1:8" ht="12.75">
-      <c r="A52" s="7"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="5"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" ht="12.75">
       <c r="A53" s="7"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
       <c r="F53" s="9"/>
@@ -1935,25 +2017,25 @@
       <c r="B54" s="11"/>
       <c r="C54" s="8"/>
       <c r="D54" s="9"/>
-      <c r="E54" s="13"/>
+      <c r="E54" s="10"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="5"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+    </row>
+    <row r="55" spans="1:8" ht="12.75">
+      <c r="A55" s="7"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" ht="12.75">
       <c r="A56" s="7"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="9"/>
       <c r="E56" s="10"/>
       <c r="F56" s="9"/>
@@ -1963,7 +2045,7 @@
     <row r="57" spans="1:8" ht="12.75">
       <c r="A57" s="7"/>
       <c r="B57" s="11"/>
-      <c r="C57" s="8"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="9"/>
       <c r="E57" s="10"/>
       <c r="F57" s="9"/>
@@ -1973,56 +2055,56 @@
     <row r="58" spans="1:8" ht="12.75">
       <c r="A58" s="7"/>
       <c r="B58" s="11"/>
-      <c r="C58" s="8"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="9"/>
-      <c r="E58" s="10"/>
+      <c r="E58" s="13"/>
       <c r="F58" s="9"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:8" ht="12.75">
       <c r="A59" s="7"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
       <c r="D59" s="9"/>
-      <c r="E59" s="10"/>
+      <c r="E59" s="13"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:8" ht="12.75">
       <c r="A60" s="7"/>
       <c r="B60" s="11"/>
-      <c r="C60" s="8"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="9"/>
-      <c r="E60" s="13"/>
+      <c r="E60" s="10"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="5"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-    </row>
-    <row r="62" spans="1:8" ht="12.75">
-      <c r="A62" s="7"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="1:8" ht="12.75">
+      <c r="A61" s="7"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="5"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
     </row>
     <row r="63" spans="1:8" ht="12.75">
       <c r="A63" s="7"/>
-      <c r="B63" s="11"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="10"/>
@@ -2043,7 +2125,7 @@
     <row r="65" spans="1:8" ht="12.75">
       <c r="A65" s="7"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
+      <c r="C65" s="8"/>
       <c r="D65" s="9"/>
       <c r="E65" s="10"/>
       <c r="F65" s="9"/>
@@ -2065,10 +2147,10 @@
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
       <c r="D67" s="9"/>
-      <c r="E67" s="13"/>
+      <c r="E67" s="10"/>
       <c r="F67" s="9"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
     </row>
     <row r="68" spans="1:8" ht="12.75">
       <c r="A68" s="7"/>
@@ -2100,39 +2182,39 @@
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="5"/>
-      <c r="B71" s="36"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
+    <row r="71" spans="1:8" ht="12.75">
+      <c r="A71" s="7"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
     </row>
     <row r="72" spans="1:8" ht="12.75">
       <c r="A72" s="7"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
       <c r="D72" s="9"/>
       <c r="E72" s="10"/>
       <c r="F72" s="9"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="1:8" ht="12.75">
-      <c r="A73" s="7"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="10"/>
-      <c r="H73" s="10"/>
+    <row r="73" spans="1:8">
+      <c r="A73" s="5"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:8" ht="12.75">
       <c r="A74" s="7"/>
-      <c r="B74" s="11"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="8"/>
       <c r="D74" s="9"/>
       <c r="E74" s="10"/>
@@ -2165,10 +2247,10 @@
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
       <c r="D77" s="9"/>
-      <c r="E77" s="13"/>
+      <c r="E77" s="10"/>
       <c r="F77" s="9"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
     </row>
     <row r="78" spans="1:8" ht="12.75">
       <c r="A78" s="7"/>
@@ -2190,150 +2272,150 @@
       <c r="G79" s="10"/>
       <c r="H79" s="10"/>
     </row>
-    <row r="80" spans="1:8" ht="12.75">
-      <c r="A80" s="7"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="10"/>
-      <c r="H80" s="10"/>
+    <row r="80" spans="1:8">
+      <c r="A80" s="5"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
     </row>
     <row r="81" spans="1:8" ht="12.75">
       <c r="A81" s="7"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="8"/>
       <c r="D81" s="9"/>
       <c r="E81" s="10"/>
       <c r="F81" s="9"/>
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="5"/>
-      <c r="B82" s="36"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
-      <c r="H82" s="6"/>
+    <row r="82" spans="1:8" ht="12.75">
+      <c r="A82" s="7"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
     </row>
     <row r="83" spans="1:8" ht="12.75">
       <c r="A83" s="7"/>
-      <c r="B83" s="8"/>
+      <c r="B83" s="12"/>
       <c r="C83" s="8"/>
       <c r="D83" s="9"/>
       <c r="E83" s="10"/>
       <c r="F83" s="9"/>
-      <c r="G83" s="10"/>
-      <c r="H83" s="10"/>
-    </row>
-    <row r="84" spans="1:8" ht="12.75">
-      <c r="A84" s="7"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="10"/>
-      <c r="H84" s="10"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="5"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
     </row>
     <row r="85" spans="1:8" ht="12.75">
       <c r="A85" s="7"/>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
       <c r="D85" s="9"/>
-      <c r="E85" s="10"/>
+      <c r="E85" s="16"/>
       <c r="F85" s="9"/>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
     </row>
     <row r="86" spans="1:8" ht="12.75">
       <c r="A86" s="7"/>
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
       <c r="D86" s="9"/>
-      <c r="E86" s="10"/>
+      <c r="E86" s="16"/>
       <c r="F86" s="9"/>
-      <c r="G86" s="10"/>
-      <c r="H86" s="10"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
     </row>
     <row r="87" spans="1:8" ht="12.75">
       <c r="A87" s="7"/>
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
       <c r="D87" s="9"/>
-      <c r="E87" s="10"/>
+      <c r="E87" s="16"/>
       <c r="F87" s="9"/>
-      <c r="G87" s="10"/>
-      <c r="H87" s="10"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
     </row>
     <row r="88" spans="1:8" ht="12.75">
       <c r="A88" s="7"/>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
       <c r="D88" s="9"/>
-      <c r="E88" s="10"/>
+      <c r="E88" s="16"/>
       <c r="F88" s="9"/>
-      <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="5"/>
-      <c r="B89" s="36"/>
-      <c r="C89" s="37"/>
-      <c r="D89" s="37"/>
-      <c r="E89" s="6"/>
-      <c r="F89" s="6"/>
-      <c r="G89" s="6"/>
-      <c r="H89" s="6"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+    </row>
+    <row r="89" spans="1:8" ht="12.75">
+      <c r="A89" s="7"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="16"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
     </row>
     <row r="90" spans="1:8" ht="12.75">
       <c r="A90" s="7"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="8"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
       <c r="D90" s="9"/>
-      <c r="E90" s="10"/>
+      <c r="E90" s="16"/>
       <c r="F90" s="9"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
     </row>
     <row r="91" spans="1:8" ht="12.75">
       <c r="A91" s="7"/>
-      <c r="B91" s="12"/>
-      <c r="C91" s="8"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="11"/>
       <c r="D91" s="9"/>
-      <c r="E91" s="10"/>
+      <c r="E91" s="16"/>
       <c r="F91" s="9"/>
-      <c r="G91" s="10"/>
-      <c r="H91" s="10"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
     </row>
     <row r="92" spans="1:8" ht="12.75">
       <c r="A92" s="7"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="8"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
       <c r="D92" s="9"/>
-      <c r="E92" s="10"/>
+      <c r="E92" s="16"/>
       <c r="F92" s="9"/>
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
     </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="5"/>
-      <c r="B93" s="36"/>
-      <c r="C93" s="37"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="15"/>
-      <c r="F93" s="6"/>
+    <row r="93" spans="1:8" ht="12.75">
+      <c r="A93" s="7"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="16"/>
+      <c r="F93" s="9"/>
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
     </row>
     <row r="94" spans="1:8" ht="12.75">
       <c r="A94" s="7"/>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
       <c r="D94" s="9"/>
       <c r="E94" s="16"/>
       <c r="F94" s="9"/>
@@ -2365,7 +2447,7 @@
       <c r="B97" s="11"/>
       <c r="C97" s="11"/>
       <c r="D97" s="9"/>
-      <c r="E97" s="16"/>
+      <c r="E97" s="17"/>
       <c r="F97" s="9"/>
       <c r="G97" s="13"/>
       <c r="H97" s="13"/>
@@ -2373,7 +2455,7 @@
     <row r="98" spans="1:8" ht="12.75">
       <c r="A98" s="7"/>
       <c r="B98" s="11"/>
-      <c r="C98" s="8"/>
+      <c r="C98" s="11"/>
       <c r="D98" s="9"/>
       <c r="E98" s="16"/>
       <c r="F98" s="9"/>
@@ -2385,7 +2467,7 @@
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
       <c r="D99" s="9"/>
-      <c r="E99" s="16"/>
+      <c r="E99" s="17"/>
       <c r="F99" s="9"/>
       <c r="G99" s="13"/>
       <c r="H99" s="13"/>
@@ -2405,176 +2487,100 @@
       <c r="B101" s="11"/>
       <c r="C101" s="11"/>
       <c r="D101" s="9"/>
-      <c r="E101" s="16"/>
+      <c r="E101" s="17"/>
       <c r="F101" s="9"/>
       <c r="G101" s="13"/>
       <c r="H101" s="13"/>
     </row>
-    <row r="102" spans="1:8" ht="12.75">
-      <c r="A102" s="7"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="9"/>
-      <c r="E102" s="16"/>
-      <c r="F102" s="9"/>
-      <c r="G102" s="13"/>
-      <c r="H102" s="13"/>
-    </row>
-    <row r="103" spans="1:8" ht="12.75">
-      <c r="A103" s="7"/>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="9"/>
-      <c r="E103" s="16"/>
-      <c r="F103" s="9"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="13"/>
-    </row>
-    <row r="104" spans="1:8" ht="12.75">
-      <c r="A104" s="7"/>
-      <c r="B104" s="11"/>
-      <c r="C104" s="11"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="16"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="13"/>
-      <c r="H104" s="13"/>
-    </row>
-    <row r="105" spans="1:8" ht="12.75">
-      <c r="A105" s="7"/>
-      <c r="B105" s="11"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="9"/>
-      <c r="E105" s="16"/>
-      <c r="F105" s="9"/>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-    </row>
-    <row r="106" spans="1:8" ht="12.75">
-      <c r="A106" s="7"/>
-      <c r="B106" s="11"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="9"/>
-      <c r="E106" s="17"/>
-      <c r="F106" s="9"/>
-      <c r="G106" s="13"/>
-      <c r="H106" s="13"/>
-    </row>
-    <row r="107" spans="1:8" ht="12.75">
-      <c r="A107" s="7"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="16"/>
-      <c r="F107" s="9"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
-    </row>
-    <row r="108" spans="1:8" ht="12.75">
-      <c r="A108" s="7"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="17"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-    </row>
-    <row r="109" spans="1:8" ht="12.75">
-      <c r="A109" s="7"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="9"/>
-      <c r="E109" s="16"/>
-      <c r="F109" s="9"/>
-      <c r="G109" s="13"/>
-      <c r="H109" s="13"/>
-    </row>
-    <row r="110" spans="1:8" ht="12.75">
-      <c r="A110" s="7"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="9"/>
-      <c r="E110" s="17"/>
-      <c r="F110" s="9"/>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13"/>
-    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B93:D93"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B82:D82"/>
+  <mergeCells count="9">
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B73:D73"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D25:D26 F25:F26 D28:D35 F28:F35 D37:D43 F37:F43 D45:D48 F45:F48 D50:D54 F50:F54 D56:D60 F56:F60 D62:D70 F62:F70 D72:D81 F72:F81 D83:D88 F83:F88 D90:D92 F90:F110 D94:D110 D16:D17 F16:F17 H16:H17">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Pass">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D28:D34 F28:F34 D36:D39 F36:F39 D41:D45 F41:F45 D47:D51 F47:F51 D53:D61 F53:F61 D63:D72 F63:F72 D74:D79 F74:F79 D81:D83 F81:F101 D85:D101 D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D25:D26 F25:F26 D28:D35 F28:F35 D37:D43 F37:F43 D45:D48 F45:F48 D50:D54 F50:F54 D56:D60 F56:F60 D62:D70 F62:F70 D72:D81 F72:F81 D83:D88 F83:F88 D90:D92 F90:F110 D94:D110 D16:D17 F16:F17 H16:H17">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D28:D34 F28:F34 D36:D39 F36:F39 D41:D45 F41:F45 D47:D51 F47:F51 D53:D61 F53:F61 D63:D72 F63:F72 D74:D79 F74:F79 D81:D83 F81:F101 D85:D101 D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D25:D26 F25:F26 D28:D35 F28:F35 D37:D43 F37:F43 D45:D48 F45:F48 D50:D54 F50:F54 D56:D60 F56:F60 D62:D70 F62:F70 D72:D81 F72:F81 D83:D88 F83:F88 D90:D92 F90:F110 D94:D110 D16:D17 F16:F17 H16:H17">
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Block / Skip">
+  <conditionalFormatting sqref="D4:D8 F4:F8 H4:H8 D28:D34 F28:F34 D36:D39 F36:F39 D41:D45 F41:F45 D47:D51 F47:F51 D53:D61 F53:F61 D63:D72 F63:F72 D74:D79 F74:F79 D81:D83 F81:F101 D85:D101 D16:D17 F16:F17 H16:H17">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14 F10:F14 H10:H14">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:D20 F19:F20 H19:H20">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D19))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:D20 F19:F20 H19:H20">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D19))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:D20 F19:F20 H19:H20">
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D19))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D23 F21:F23 H21:H23">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D21))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D23 F21:F23 H21:H23">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D21))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D23 F21:F23 H21:H23">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D21))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D25:D26 F25:F26 H25:H26">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:D26 F25:F26 H25:H26">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:D26 F25:F26 H25:H26">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D8 F4:F8 H4:H8 F90:F92 D94:D110 F94:F110 D83:D88 F83:F88 D90:D92 H10:H14 F10:F14 D10:D14 D25:D26 F25:F26 D28:D35 F28:F35 D37:D43 F37:F43 D45:D48 F45:F48 D50:D54 F50:F54 D56:D60 F56:F60 D62:D70 F62:F70 D72:D81 F72:F81 D19:D23 H19:H23 F19:F23 F16:F17 H16:H17 D16:D17" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D8 F4:F8 H4:H8 F81:F83 D85:D101 F85:F101 D74:D79 F74:F79 D81:D83 H10:H14 F10:F14 D10:D14 H16:H17 D16:D17 D28:D34 F28:F34 D36:D39 F36:F39 D41:D45 F41:F45 D47:D51 F47:F51 D53:D61 F53:F61 D63:D72 F63:F72 D19:D23 H19:H23 F19:F23 F16:F17 D25:D26 F25:F26 H25:H26" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>